<commit_message>
Updated model results and comparaison
</commit_message>
<xml_diff>
--- a/nnet/results.xlsx
+++ b/nnet/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IHAbB\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IHAbB\Documents\Code\_srs\visual-relationship-caption2\nnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B150DFD5-349B-4C8A-95C9-AE4B79CCF702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4CEE3B-689D-4CF3-B11C-30B706CCE4AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8895" yWindow="2610" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="16">
   <si>
     <t>inception_v3</t>
   </si>
@@ -55,6 +55,27 @@
   </si>
   <si>
     <t>vgg19</t>
+  </si>
+  <si>
+    <t>image_model</t>
+  </si>
+  <si>
+    <t>number_layers</t>
+  </si>
+  <si>
+    <t>train_validation</t>
+  </si>
+  <si>
+    <t>correct_prediction</t>
+  </si>
+  <si>
+    <t>total_images</t>
+  </si>
+  <si>
+    <t>total_relations</t>
+  </si>
+  <si>
+    <t>recall@100</t>
   </si>
 </sst>
 </file>
@@ -896,39 +917,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>45609</v>
-      </c>
-      <c r="E1">
-        <v>51487</v>
-      </c>
-      <c r="F1" s="1">
-        <f>D1/E1</f>
-        <v>0.88583525938586438</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -936,41 +962,45 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>4951</v>
+        <v>45609</v>
       </c>
       <c r="E2">
-        <v>5700</v>
-      </c>
-      <c r="F2" s="1">
-        <f t="shared" ref="F2:F38" si="0">D2/E2</f>
-        <v>0.86859649122807014</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F2">
+        <v>174106</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.26200000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>42190</v>
+        <v>4951</v>
       </c>
       <c r="E3">
-        <v>51487</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>0.81943014741585252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F3">
+        <v>39683</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.12479999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -978,41 +1008,45 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>4688</v>
+        <v>42190</v>
       </c>
       <c r="E4">
-        <v>5700</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>0.82245614035087722</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F4">
+        <v>174106</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.24229999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>46471</v>
+        <v>4688</v>
       </c>
       <c r="E5">
-        <v>51487</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>0.90257734962223479</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F5">
+        <v>39683</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.1181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1020,41 +1054,45 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>46471</v>
+      </c>
+      <c r="E6">
+        <v>51487</v>
+      </c>
+      <c r="F6">
+        <v>174106</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.26690000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>5019</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>5700</v>
       </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.88052631578947371</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>48270</v>
-      </c>
-      <c r="E7">
-        <v>51487</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.93751820847981049</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>39683</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.1265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1062,41 +1100,45 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>5180</v>
+        <v>48270</v>
       </c>
       <c r="E8">
-        <v>5700</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.90877192982456145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F8">
+        <v>174106</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.2772</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>50352</v>
+        <v>5180</v>
       </c>
       <c r="E9">
-        <v>51487</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.97795560044283025</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F9">
+        <v>39683</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.1305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1104,41 +1146,45 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>5575</v>
+        <v>50352</v>
       </c>
       <c r="E10">
-        <v>5700</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.97807017543859653</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F10">
+        <v>174106</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.28920000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>50218</v>
+        <v>5575</v>
       </c>
       <c r="E11">
-        <v>51487</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>0.97535300172859163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F11">
+        <v>39683</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.14050000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1146,41 +1192,45 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>50218</v>
+      </c>
+      <c r="E12">
+        <v>51487</v>
+      </c>
+      <c r="F12">
+        <v>174106</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.28839999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>5540</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>5700</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.97192982456140353</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>47742</v>
-      </c>
-      <c r="E13">
-        <v>51487</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.927263192650572</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>39683</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.1396</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1188,41 +1238,45 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>5285</v>
+        <v>47742</v>
       </c>
       <c r="E14">
-        <v>5700</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.92719298245614035</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F14">
+        <v>174106</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.2742</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>49768</v>
+        <v>5285</v>
       </c>
       <c r="E15">
-        <v>51487</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>0.9666129314195816</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F15">
+        <v>39683</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.13320000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1230,41 +1284,45 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>5442</v>
+        <v>49768</v>
       </c>
       <c r="E16">
-        <v>5700</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>0.95473684210526311</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F16">
+        <v>174106</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.2858</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>50206</v>
+        <v>5442</v>
       </c>
       <c r="E17">
-        <v>51487</v>
-      </c>
-      <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>0.97511993318701806</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F17">
+        <v>39683</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.1371</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1272,41 +1330,45 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>50206</v>
+      </c>
+      <c r="E18">
+        <v>51487</v>
+      </c>
+      <c r="F18">
+        <v>174106</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.28839999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>5532</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>5700</v>
       </c>
-      <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>0.97052631578947368</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>21356</v>
-      </c>
-      <c r="E19">
-        <v>51487</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>0.41478431448715208</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>39683</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.1394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1314,41 +1376,45 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>2534</v>
+        <v>21356</v>
       </c>
       <c r="E20">
-        <v>5700</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>0.44456140350877194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F20">
+        <v>174106</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.1227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>18884</v>
+        <v>2534</v>
       </c>
       <c r="E21">
-        <v>51487</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>0.36677219492299029</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F21">
+        <v>39683</v>
+      </c>
+      <c r="G21" s="1">
+        <v>6.3899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1356,41 +1422,45 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>2505</v>
+        <v>18884</v>
       </c>
       <c r="E22">
-        <v>5700</v>
-      </c>
-      <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>0.43947368421052629</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F22">
+        <v>174106</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.1085</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>21126</v>
+        <v>2505</v>
       </c>
       <c r="E23">
-        <v>51487</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>0.41031716744032476</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F23">
+        <v>39683</v>
+      </c>
+      <c r="G23" s="1">
+        <v>6.3100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1398,41 +1468,45 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>21126</v>
+      </c>
+      <c r="E24">
+        <v>51487</v>
+      </c>
+      <c r="F24">
+        <v>174106</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.12130000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
         <v>2</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>2746</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>5700</v>
       </c>
-      <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>0.48175438596491227</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>18064</v>
-      </c>
-      <c r="E25">
-        <v>51487</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" si="0"/>
-        <v>0.35084584458212753</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>39683</v>
+      </c>
+      <c r="G25" s="1">
+        <v>6.9199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1440,41 +1514,45 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>2505</v>
+        <v>18064</v>
       </c>
       <c r="E26">
-        <v>5700</v>
-      </c>
-      <c r="F26" s="1">
-        <f t="shared" si="0"/>
-        <v>0.43947368421052629</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F26">
+        <v>174106</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.1038</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>18615</v>
+        <v>2505</v>
       </c>
       <c r="E27">
-        <v>51487</v>
-      </c>
-      <c r="F27" s="1">
-        <f t="shared" si="0"/>
-        <v>0.36154757511604874</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F27">
+        <v>39683</v>
+      </c>
+      <c r="G27" s="1">
+        <v>6.3100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1482,41 +1560,45 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>18615</v>
+      </c>
+      <c r="E28">
+        <v>51487</v>
+      </c>
+      <c r="F28">
+        <v>174106</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.1069</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
         <v>2</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>2562</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>5700</v>
       </c>
-      <c r="F28" s="1">
-        <f t="shared" si="0"/>
-        <v>0.4494736842105263</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>20046</v>
-      </c>
-      <c r="E29">
-        <v>51487</v>
-      </c>
-      <c r="F29" s="1">
-        <f t="shared" si="0"/>
-        <v>0.38934099869870065</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>39683</v>
+      </c>
+      <c r="G29" s="1">
+        <v>6.4600000000000005E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1524,41 +1606,45 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>2867</v>
+        <v>20046</v>
       </c>
       <c r="E30">
-        <v>5700</v>
-      </c>
-      <c r="F30" s="1">
-        <f t="shared" si="0"/>
-        <v>0.50298245614035086</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F30">
+        <v>174106</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.11509999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
       <c r="B31">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>21984</v>
+        <v>2867</v>
       </c>
       <c r="E31">
-        <v>51487</v>
-      </c>
-      <c r="F31" s="1">
-        <f t="shared" si="0"/>
-        <v>0.42698156816283722</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F31">
+        <v>39683</v>
+      </c>
+      <c r="G31" s="1">
+        <v>7.22E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1566,41 +1652,45 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>21984</v>
+      </c>
+      <c r="E32">
+        <v>51487</v>
+      </c>
+      <c r="F32">
+        <v>174106</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.1263</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
         <v>2</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>2891</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>5700</v>
       </c>
-      <c r="F32" s="1">
-        <f t="shared" si="0"/>
-        <v>0.50719298245614031</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>18619</v>
-      </c>
-      <c r="E33">
-        <v>51487</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="0"/>
-        <v>0.36162526462990657</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>39683</v>
+      </c>
+      <c r="G33" s="1">
+        <v>7.2900000000000006E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1608,41 +1698,45 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>2624</v>
+        <v>18619</v>
       </c>
       <c r="E34">
-        <v>5700</v>
-      </c>
-      <c r="F34" s="1">
-        <f t="shared" si="0"/>
-        <v>0.46035087719298246</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F34">
+        <v>174106</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.1069</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
       <c r="B35">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>18958</v>
+        <v>2624</v>
       </c>
       <c r="E35">
-        <v>51487</v>
-      </c>
-      <c r="F35" s="1">
-        <f t="shared" si="0"/>
-        <v>0.3682094509293608</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F35">
+        <v>39683</v>
+      </c>
+      <c r="G35" s="1">
+        <v>6.6100000000000006E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1650,41 +1744,45 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>2691</v>
+        <v>18958</v>
       </c>
       <c r="E36">
-        <v>5700</v>
-      </c>
-      <c r="F36" s="1">
-        <f t="shared" si="0"/>
-        <v>0.47210526315789475</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51487</v>
+      </c>
+      <c r="F36">
+        <v>174106</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.1089</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
       <c r="B37">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37">
-        <v>20115</v>
+        <v>2691</v>
       </c>
       <c r="E37">
-        <v>51487</v>
-      </c>
-      <c r="F37" s="1">
-        <f t="shared" si="0"/>
-        <v>0.39068114281274885</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+      <c r="F37">
+        <v>39683</v>
+      </c>
+      <c r="G37" s="1">
+        <v>6.7799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1692,21 +1790,56 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>20115</v>
+      </c>
+      <c r="E38">
+        <v>51487</v>
+      </c>
+      <c r="F38">
+        <v>174106</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.11550000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
         <v>2</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>2759</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>5700</v>
       </c>
-      <c r="F38" s="1">
-        <f t="shared" si="0"/>
-        <v>0.48403508771929826</v>
+      <c r="F39">
+        <v>39683</v>
+      </c>
+      <c r="G39" s="1">
+        <v>6.9500000000000006E-2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576">
+  <conditionalFormatting sqref="F40:F1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G39">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>